<commit_message>
zotero metadata retrieval handling item missing case
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_detectlimit.xlsx
+++ b/nbs/files/lut/dbo_detectlimit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC2BCCE-B1E3-2D4E-85BF-4C444B16E028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1039B97F-5308-CC40-AF73-650F72B989B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2500" windowWidth="26440" windowHeight="14940" xr2:uid="{0CCB2E01-F9A9-4C41-96E9-A4609841CF4C}"/>
+    <workbookView xWindow="2120" yWindow="3060" windowWidth="26440" windowHeight="14940" xr2:uid="{0CCB2E01-F9A9-4C41-96E9-A4609841CF4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>=</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Derived</t>
+  </si>
+  <si>
+    <t>Not available</t>
+  </si>
+  <si>
+    <t>Not Available</t>
   </si>
 </sst>
 </file>
@@ -430,11 +436,12 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -454,10 +461,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -465,10 +472,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -476,10 +483,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -487,13 +494,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
       <c r="I6" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add sanitized names fo detect limit and unit
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_detectlimit.xlsx
+++ b/nbs/files/lut/dbo_detectlimit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5438ECCF-CE02-914C-891F-A1B46C984563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC2DDE8-5509-5D44-8B82-F83FFF8C22BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="3060" windowWidth="26440" windowHeight="14940" xr2:uid="{0CCB2E01-F9A9-4C41-96E9-A4609841CF4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>=</t>
   </si>
@@ -439,7 +439,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,6 +466,9 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">

</xml_diff>